<commit_message>
added list by section and make the file as one
</commit_message>
<xml_diff>
--- a/src/Form-3-ENROLLMENT-LIST-FORMAT.xlsx
+++ b/src/Form-3-ENROLLMENT-LIST-FORMAT.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>FORM 3 - Enrollment List Format- CHED RMO No. 22, s. 2021  effective AY 2021-2022</t>
   </si>
@@ -95,18 +95,6 @@
   </si>
   <si>
     <t>MALE/FEMALE</t>
-  </si>
-  <si>
-    <t>PREPARED BY:</t>
-  </si>
-  <si>
-    <t>CERTIFIED CORRECT BY:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NAME OF REGISTRAR </t>
-  </si>
-  <si>
-    <t xml:space="preserve">POSITION </t>
   </si>
 </sst>
 </file>
@@ -255,6 +243,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -275,13 +270,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -608,8 +596,8 @@
   </sheetPr>
   <dimension ref="A1:R40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+    <sheetView tabSelected="1" topLeftCell="H7" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="R8" sqref="R8:R9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -626,16 +614,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="17"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="20"/>
       <c r="I1" s="6"/>
       <c r="J1" s="6"/>
       <c r="K1" s="6"/>
@@ -648,16 +636,16 @@
       <c r="R1" s="7"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="17"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="20"/>
       <c r="I2" s="9"/>
       <c r="J2" s="9"/>
       <c r="K2" s="9"/>
@@ -670,16 +658,16 @@
       <c r="R2" s="10"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="16"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
-      <c r="H3" s="17"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="20"/>
       <c r="I3" s="9"/>
       <c r="J3" s="9"/>
       <c r="K3" s="9"/>
@@ -692,14 +680,14 @@
       <c r="R3" s="10"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" s="15"/>
-      <c r="B4" s="16"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="16"/>
-      <c r="H4" s="17"/>
+      <c r="A4" s="18"/>
+      <c r="B4" s="19"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="20"/>
       <c r="I4" s="9"/>
       <c r="J4" s="9"/>
       <c r="K4" s="9"/>
@@ -716,12 +704,12 @@
         <v>3</v>
       </c>
       <c r="B5" s="3"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="16"/>
-      <c r="H5" s="17"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="20"/>
       <c r="I5" s="9"/>
       <c r="J5" s="9"/>
       <c r="K5" s="9"/>
@@ -734,18 +722,18 @@
       <c r="R5" s="10"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A6" s="20" t="s">
+      <c r="A6" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="17"/>
+      <c r="B6" s="20"/>
       <c r="C6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="18"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="17"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="20"/>
       <c r="I6" s="9"/>
       <c r="J6" s="9"/>
       <c r="K6" s="9"/>
@@ -758,14 +746,14 @@
       <c r="R6" s="10"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A7" s="18"/>
-      <c r="B7" s="16"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="16"/>
-      <c r="H7" s="17"/>
+      <c r="A7" s="21"/>
+      <c r="B7" s="19"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="20"/>
       <c r="I7" s="9"/>
       <c r="J7" s="9"/>
       <c r="K7" s="9"/>
@@ -778,19 +766,19 @@
       <c r="R7" s="10"/>
     </row>
     <row r="8" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="15" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="12" t="s">
+      <c r="E8" s="15" t="s">
         <v>10</v>
       </c>
       <c r="F8" s="8" t="s">
@@ -799,66 +787,64 @@
       <c r="G8" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="H8" s="12" t="s">
+      <c r="H8" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="I8" s="12" t="s">
+      <c r="I8" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="J8" s="12" t="s">
+      <c r="J8" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="K8" s="12" t="s">
+      <c r="K8" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="L8" s="12" t="s">
+      <c r="L8" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="M8" s="12" t="s">
+      <c r="M8" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="N8" s="12" t="s">
+      <c r="N8" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="O8" s="12" t="s">
+      <c r="O8" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="P8" s="12" t="s">
+      <c r="P8" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="Q8" s="12" t="s">
+      <c r="Q8" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="R8" s="14" t="s">
+      <c r="R8" s="17" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="13"/>
-      <c r="B9" s="13"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
+      <c r="A9" s="16"/>
+      <c r="B9" s="16"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
       <c r="F9" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="G9" s="13"/>
-      <c r="H9" s="13"/>
-      <c r="I9" s="13"/>
-      <c r="J9" s="13"/>
-      <c r="K9" s="13"/>
-      <c r="L9" s="13"/>
-      <c r="M9" s="13"/>
-      <c r="N9" s="13"/>
-      <c r="O9" s="13"/>
-      <c r="P9" s="13"/>
-      <c r="Q9" s="13"/>
-      <c r="R9" s="13"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="16"/>
+      <c r="J9" s="16"/>
+      <c r="K9" s="16"/>
+      <c r="L9" s="16"/>
+      <c r="M9" s="16"/>
+      <c r="N9" s="16"/>
+      <c r="O9" s="16"/>
+      <c r="P9" s="16"/>
+      <c r="Q9" s="16"/>
+      <c r="R9" s="16"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>1</v>
-      </c>
+      <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -878,9 +864,7 @@
       <c r="R10" s="1"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>2</v>
-      </c>
+      <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
@@ -900,9 +884,7 @@
       <c r="R11" s="1"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>3</v>
-      </c>
+      <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
@@ -922,9 +904,7 @@
       <c r="R12" s="1"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>4</v>
-      </c>
+      <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -944,9 +924,7 @@
       <c r="R13" s="1"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>5</v>
-      </c>
+      <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -966,9 +944,7 @@
       <c r="R14" s="1"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
-        <v>6</v>
-      </c>
+      <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
@@ -988,9 +964,7 @@
       <c r="R15" s="1"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
-        <v>7</v>
-      </c>
+      <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
@@ -1010,9 +984,7 @@
       <c r="R16" s="1"/>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
-        <v>8</v>
-      </c>
+      <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
@@ -1032,9 +1004,7 @@
       <c r="R17" s="1"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
-        <v>9</v>
-      </c>
+      <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
@@ -1054,9 +1024,7 @@
       <c r="R18" s="1"/>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
-        <v>10</v>
-      </c>
+      <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
@@ -1076,9 +1044,7 @@
       <c r="R19" s="1"/>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
-        <v>11</v>
-      </c>
+      <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
@@ -1098,9 +1064,7 @@
       <c r="R20" s="1"/>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
-        <v>12</v>
-      </c>
+      <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
@@ -1120,9 +1084,7 @@
       <c r="R21" s="1"/>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
-        <v>13</v>
-      </c>
+      <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
@@ -1142,9 +1104,7 @@
       <c r="R22" s="1"/>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A23" s="1">
-        <v>14</v>
-      </c>
+      <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
@@ -1164,9 +1124,7 @@
       <c r="R23" s="1"/>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A24" s="1">
-        <v>15</v>
-      </c>
+      <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
@@ -1186,9 +1144,7 @@
       <c r="R24" s="1"/>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A25" s="1">
-        <v>16</v>
-      </c>
+      <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
@@ -1208,9 +1164,7 @@
       <c r="R25" s="1"/>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A26" s="1">
-        <v>17</v>
-      </c>
+      <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
@@ -1230,9 +1184,7 @@
       <c r="R26" s="1"/>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A27" s="1">
-        <v>18</v>
-      </c>
+      <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
@@ -1252,9 +1204,7 @@
       <c r="R27" s="1"/>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A28" s="1">
-        <v>19</v>
-      </c>
+      <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
@@ -1274,9 +1224,7 @@
       <c r="R28" s="1"/>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A29" s="1">
-        <v>20</v>
-      </c>
+      <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
@@ -1296,9 +1244,7 @@
       <c r="R29" s="1"/>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A30" s="1">
-        <v>21</v>
-      </c>
+      <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
@@ -1318,9 +1264,7 @@
       <c r="R30" s="1"/>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A31" s="1">
-        <v>22</v>
-      </c>
+      <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
@@ -1340,9 +1284,7 @@
       <c r="R31" s="1"/>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A32" s="1">
-        <v>23</v>
-      </c>
+      <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
@@ -1362,9 +1304,7 @@
       <c r="R32" s="1"/>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A33" s="1">
-        <v>24</v>
-      </c>
+      <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
@@ -1384,9 +1324,7 @@
       <c r="R33" s="1"/>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A34" s="1">
-        <v>25</v>
-      </c>
+      <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
@@ -1406,9 +1344,7 @@
       <c r="R34" s="1"/>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A35" s="1">
-        <v>26</v>
-      </c>
+      <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
@@ -1428,43 +1364,47 @@
       <c r="R35" s="1"/>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A37" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="B37" s="22"/>
-      <c r="C37" s="22"/>
-      <c r="D37" s="22"/>
-      <c r="E37" s="22"/>
-      <c r="G37" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="H37" s="22"/>
+      <c r="A37" s="12"/>
+      <c r="B37" s="13"/>
+      <c r="C37" s="13"/>
+      <c r="D37" s="13"/>
+      <c r="E37" s="13"/>
+      <c r="F37" s="13"/>
+      <c r="G37" s="12"/>
+      <c r="H37" s="13"/>
+    </row>
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A38" s="13"/>
+      <c r="B38" s="13"/>
+      <c r="C38" s="13"/>
+      <c r="D38" s="13"/>
+      <c r="E38" s="13"/>
+      <c r="F38" s="13"/>
+      <c r="G38" s="13"/>
+      <c r="H38" s="13"/>
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="G39" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="H39" s="22"/>
+      <c r="A39" s="13"/>
+      <c r="B39" s="13"/>
+      <c r="C39" s="13"/>
+      <c r="D39" s="13"/>
+      <c r="E39" s="13"/>
+      <c r="F39" s="13"/>
+      <c r="G39" s="14"/>
+      <c r="H39" s="13"/>
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="G40" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="H40" s="22"/>
+      <c r="A40" s="13"/>
+      <c r="B40" s="13"/>
+      <c r="C40" s="13"/>
+      <c r="D40" s="13"/>
+      <c r="E40" s="13"/>
+      <c r="F40" s="13"/>
+      <c r="G40" s="14"/>
+      <c r="H40" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="29">
-    <mergeCell ref="A37:E37"/>
-    <mergeCell ref="G37:H37"/>
-    <mergeCell ref="G39:H39"/>
-    <mergeCell ref="G40:H40"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="H8:H9"/>
+  <mergeCells count="25">
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="A4:H4"/>
     <mergeCell ref="A6:B6"/>
@@ -1477,6 +1417,13 @@
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A3:H3"/>
     <mergeCell ref="A7:H7"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="H8:H9"/>
     <mergeCell ref="P8:P9"/>
     <mergeCell ref="Q8:Q9"/>
     <mergeCell ref="R8:R9"/>

</xml_diff>